<commit_message>
Updated tasks for EDA
</commit_message>
<xml_diff>
--- a/EDA_tasks.xlsx
+++ b/EDA_tasks.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="46">
   <si>
     <t>Task</t>
   </si>
@@ -67,13 +67,166 @@
   </si>
   <si>
     <t>Sr. No.</t>
+  </si>
+  <si>
+    <t>High Interest Loans</t>
+  </si>
+  <si>
+    <t>How many loans have high interest loans?</t>
+  </si>
+  <si>
+    <t>Loan Grade counts</t>
+  </si>
+  <si>
+    <t>Level</t>
+  </si>
+  <si>
+    <t>How many loan count under each grade?</t>
+  </si>
+  <si>
+    <t>Loan Status</t>
+  </si>
+  <si>
+    <t>What are the different loan status and their count map</t>
+  </si>
+  <si>
+    <t>high</t>
+  </si>
+  <si>
+    <t>low</t>
+  </si>
+  <si>
+    <t>medium</t>
+  </si>
+  <si>
+    <t>Economic Profiling</t>
+  </si>
+  <si>
+    <t>Application type</t>
+  </si>
+  <si>
+    <t>How many applications with different count type?</t>
+  </si>
+  <si>
+    <t>Annual income vs application type</t>
+  </si>
+  <si>
+    <t>Plot annual vs application type graph - Violin plot</t>
+  </si>
+  <si>
+    <t>Check relationship between income and loan amount - Box plot</t>
+  </si>
+  <si>
+    <t>Income vs loan amount</t>
+  </si>
+  <si>
+    <t>Income vs loan grades</t>
+  </si>
+  <si>
+    <t>Check relationship between income and loan grades - Box plot</t>
+  </si>
+  <si>
+    <t>Employment title</t>
+  </si>
+  <si>
+    <t>Histogram for various employement titles</t>
+  </si>
+  <si>
+    <t>Annual income vs Emp title</t>
+  </si>
+  <si>
+    <t>Check relationship between income and top emp titles - Box plot</t>
+  </si>
+  <si>
+    <t>Ninja Loans</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Check how many people with no job no income no assests got loan </t>
+  </si>
+  <si>
+    <t>Annual income(&gt;100/&gt;120$) vs Emp title</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Its important to undestand what kind of public we are dealing with ------
+Income</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">: annual income in USD
+</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Employment Length-stability</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">: how many years of employment at the current job.
+</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Employment Title</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>: job title provided by the borrower in the loan application
+We will analyze each of these variables and how they interact within our dataset.</t>
+    </r>
+  </si>
+  <si>
+    <t>Applications vs Emp length &gt;10y</t>
+  </si>
+  <si>
+    <t>Check how many people have 10years of employment left</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -89,6 +242,14 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -98,7 +259,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="15">
     <border>
       <left/>
       <right/>
@@ -106,14 +267,236 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="27">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -415,10 +798,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C8"/>
+  <dimension ref="A1:D24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+      <selection activeCell="G16" sqref="G16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -427,95 +810,323 @@
     <col min="3" max="3" width="86.88671875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A1" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="7" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A2">
+      <c r="D1" s="8" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A2" s="9">
         <v>1</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="C2" t="s">
+      <c r="C2" s="3" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A3">
+      <c r="D2" s="10" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A3" s="9">
         <v>2</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B3" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="C3" t="s">
+      <c r="C3" s="3" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A4">
+      <c r="D3" s="10" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A4" s="9">
         <v>3</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B4" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="C4" t="s">
+      <c r="C4" s="3" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A5">
+      <c r="D4" s="10" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A5" s="9">
         <v>4</v>
       </c>
-      <c r="B5" t="s">
+      <c r="B5" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="C5" t="s">
+      <c r="C5" s="3" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A6">
+      <c r="D5" s="10" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A6" s="9">
         <v>5</v>
       </c>
-      <c r="B6" t="s">
+      <c r="B6" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="C6" s="2" t="s">
+      <c r="C6" s="4" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A7">
+      <c r="D6" s="10" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A7" s="9">
         <v>6</v>
       </c>
-      <c r="B7" t="s">
+      <c r="B7" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="C7" t="s">
+      <c r="C7" s="3" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A8">
+      <c r="D7" s="10" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A8" s="9">
         <v>7</v>
       </c>
-      <c r="B8" t="s">
+      <c r="B8" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="C8" t="s">
+      <c r="C8" s="3" t="s">
         <v>9</v>
       </c>
+      <c r="D8" s="10" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A9" s="9">
+        <v>8</v>
+      </c>
+      <c r="B9" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="C9" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="D9" s="10" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A10" s="9">
+        <v>9</v>
+      </c>
+      <c r="B10" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="C10" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="D10" s="10" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A11" s="11">
+        <v>10</v>
+      </c>
+      <c r="B11" s="12" t="s">
+        <v>22</v>
+      </c>
+      <c r="C11" s="12" t="s">
+        <v>23</v>
+      </c>
+      <c r="D11" s="13" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" s="1" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A13" s="14" t="s">
+        <v>27</v>
+      </c>
+      <c r="B13" s="15"/>
+      <c r="C13" s="15"/>
+      <c r="D13" s="16"/>
+    </row>
+    <row r="14" spans="1:4" ht="81" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A14" s="17" t="s">
+        <v>43</v>
+      </c>
+      <c r="B14" s="5"/>
+      <c r="C14" s="5"/>
+      <c r="D14" s="18"/>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A15" s="19" t="s">
+        <v>16</v>
+      </c>
+      <c r="B15" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C15" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="D15" s="20" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A16" s="21">
+        <v>1</v>
+      </c>
+      <c r="B16" s="22" t="s">
+        <v>28</v>
+      </c>
+      <c r="C16" s="22" t="s">
+        <v>29</v>
+      </c>
+      <c r="D16" s="23" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A17" s="21">
+        <v>2</v>
+      </c>
+      <c r="B17" s="22" t="s">
+        <v>30</v>
+      </c>
+      <c r="C17" s="22" t="s">
+        <v>31</v>
+      </c>
+      <c r="D17" s="23" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A18" s="21">
+        <v>3</v>
+      </c>
+      <c r="B18" s="22" t="s">
+        <v>33</v>
+      </c>
+      <c r="C18" s="22" t="s">
+        <v>32</v>
+      </c>
+      <c r="D18" s="23" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A19" s="21">
+        <v>4</v>
+      </c>
+      <c r="B19" s="22" t="s">
+        <v>34</v>
+      </c>
+      <c r="C19" s="22" t="s">
+        <v>35</v>
+      </c>
+      <c r="D19" s="23" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A20" s="21">
+        <v>5</v>
+      </c>
+      <c r="B20" s="22" t="s">
+        <v>36</v>
+      </c>
+      <c r="C20" s="22" t="s">
+        <v>37</v>
+      </c>
+      <c r="D20" s="23" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A21" s="21">
+        <v>6</v>
+      </c>
+      <c r="B21" s="22" t="s">
+        <v>38</v>
+      </c>
+      <c r="C21" s="22" t="s">
+        <v>39</v>
+      </c>
+      <c r="D21" s="23" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A22" s="21">
+        <v>7</v>
+      </c>
+      <c r="B22" s="22" t="s">
+        <v>42</v>
+      </c>
+      <c r="C22" s="22" t="s">
+        <v>39</v>
+      </c>
+      <c r="D22" s="23" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A23" s="21">
+        <v>8</v>
+      </c>
+      <c r="B23" s="22" t="s">
+        <v>40</v>
+      </c>
+      <c r="C23" s="22" t="s">
+        <v>41</v>
+      </c>
+      <c r="D23" s="23" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A24" s="24">
+        <v>9</v>
+      </c>
+      <c r="B24" s="25" t="s">
+        <v>44</v>
+      </c>
+      <c r="C24" s="25" t="s">
+        <v>45</v>
+      </c>
+      <c r="D24" s="26" t="s">
+        <v>25</v>
+      </c>
     </row>
   </sheetData>
+  <mergeCells count="3">
+    <mergeCell ref="A13:D13"/>
+    <mergeCell ref="A14:D14"/>
+    <mergeCell ref="A12:XFD12"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>